<commit_message>
new functionality to compare differences between quarter data
</commit_message>
<xml_diff>
--- a/tests/resources/cut_down_master_4_2016.xlsx
+++ b/tests/resources/cut_down_master_4_2016.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t xml:space="preserve">Re-baseline HMT benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Key</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -560,6 +563,11 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="1047629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1047630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
get_project_groups first added. refactor of cost v schedule started. tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/cut_down_master_4_2016.xlsx
+++ b/tests/resources/cut_down_master_4_2016.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -143,6 +143,18 @@
   </si>
   <si>
     <t xml:space="preserve">New Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDC approval point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strategic Outline Case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Business Case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outline Business Case</t>
   </si>
 </sst>
 </file>
@@ -154,7 +166,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD\ H:MM:SS"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -183,6 +195,12 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -227,7 +245,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -249,6 +267,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,7 +298,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -567,6 +589,23 @@
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="1047629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
more ipdc_dashboard refactoring. all related tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/cut_down_master_4_2016.xlsx
+++ b/tests/resources/cut_down_master_4_2016.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -130,6 +130,9 @@
     <t xml:space="preserve">Re-baseline IPDC cost</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Re-baseline IPDC benefits</t>
   </si>
   <si>
@@ -155,6 +158,15 @@
   </si>
   <si>
     <t xml:space="preserve">Outline Business Case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMPP - IPA DCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Departmental DCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green</t>
   </si>
 </sst>
 </file>
@@ -166,7 +178,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD\ H:MM:SS"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -195,12 +207,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -245,7 +251,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -267,10 +273,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -298,7 +300,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="bottomRight" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -535,16 +537,26 @@
       <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -555,7 +567,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -566,7 +578,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -577,7 +589,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -588,24 +600,49 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
-        <v>41</v>
+      <c r="A20" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="1047629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
dandelion data added to cli
</commit_message>
<xml_diff>
--- a/tests/resources/cut_down_master_4_2016.xlsx
+++ b/tests/resources/cut_down_master_4_2016.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve">Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Forecast</t>
   </si>
 </sst>
 </file>
@@ -300,7 +303,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -643,6 +646,26 @@
       </c>
       <c r="F22" s="2" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>3067</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>89809</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>87879</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>4345</v>
       </c>
     </row>
     <row r="1047629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
further work on dandelion
</commit_message>
<xml_diff>
--- a/tests/resources/cut_down_master_4_2016.xlsx
+++ b/tests/resources/cut_down_master_4_2016.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t xml:space="preserve">Total Forecast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMPP - IPA ID Number</t>
   </si>
 </sst>
 </file>
@@ -303,7 +306,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="bottomRight" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -666,6 +669,11 @@
       </c>
       <c r="F23" s="2" t="n">
         <v>4345</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="1047629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
wp. initial code and first tests for putting data in json file
</commit_message>
<xml_diff>
--- a/tests/resources/cut_down_master_4_2016.xlsx
+++ b/tests/resources/cut_down_master_4_2016.xlsx
@@ -306,13 +306,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="59.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="996" min="2" style="2" width="8.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="2" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="996" min="6" style="2" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="997" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="2" width="9.14"/>
   </cols>
@@ -351,11 +353,11 @@
       <c r="D2" s="3" t="n">
         <v>42843</v>
       </c>
-      <c r="E2" s="4" t="n">
-        <v>42829</v>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>42832</v>
+      <c r="E2" s="3" t="n">
+        <v>42844</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>42845</v>
       </c>
       <c r="G2" s="4"/>
     </row>

</xml_diff>